<commit_message>
update database and change read_price algorithm
</commit_message>
<xml_diff>
--- a/database/industries/bargh/bemoto/balancesheet/quarterly.xlsx
+++ b/database/industries/bargh/bemoto/balancesheet/quarterly.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\bargh\bemoto\balancesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EBRAHIMI\Desktop\Trade\database\industries\bargh\bemoto\balancesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F579B5-04D1-4DFB-9114-D3C6671EF331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA03955-58F6-4640-AA59-013671F1C59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>دوره مالی</t>
   </si>
   <si>
-    <t>فصل چهارم منتهی به 1399/06</t>
-  </si>
-  <si>
     <t>فصل اول منتهی به 1399/09</t>
   </si>
   <si>
@@ -67,12 +64,12 @@
     <t>فصل اول منتهی به 1401/09</t>
   </si>
   <si>
+    <t>فصل دوم منتهی به 1401/12</t>
+  </si>
+  <si>
     <t>تاریخ انتشار</t>
   </si>
   <si>
-    <t>1400-09-10 (10)</t>
-  </si>
-  <si>
     <t>1399-10-30</t>
   </si>
   <si>
@@ -94,10 +91,13 @@
     <t>1401-04-28</t>
   </si>
   <si>
-    <t>1401-10-28 (3)</t>
+    <t>1402-02-23 (5)</t>
   </si>
   <si>
     <t>1401-10-28</t>
+  </si>
+  <si>
+    <t>1402-02-23 (2)</t>
   </si>
   <si>
     <t>دارایی</t>
@@ -732,19 +732,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="31" customWidth="1"/>
-    <col min="9" max="11" width="29" customWidth="1"/>
-    <col min="12" max="12" width="31" customWidth="1"/>
-    <col min="13" max="13" width="29" customWidth="1"/>
+    <col min="4" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="10" width="29" customWidth="1"/>
+    <col min="11" max="11" width="31" customWidth="1"/>
+    <col min="12" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -758,7 +757,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -774,7 +773,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -790,7 +789,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -804,7 +803,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:13" ht="42" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -820,7 +819,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="2:13" ht="42" x14ac:dyDescent="0.65">
+    <row r="6" spans="2:13" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -836,7 +835,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -850,7 +849,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -886,7 +885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -922,7 +921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -936,7 +935,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>26</v>
       </c>
@@ -952,43 +951,43 @@
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15">
-        <v>486836</v>
+        <v>651764</v>
       </c>
       <c r="E12" s="15">
-        <v>651764</v>
+        <v>2069976</v>
       </c>
       <c r="F12" s="15">
-        <v>2069976</v>
+        <v>457374</v>
       </c>
       <c r="G12" s="15">
-        <v>457374</v>
+        <v>249763</v>
       </c>
       <c r="H12" s="15">
-        <v>249763</v>
+        <v>609218</v>
       </c>
       <c r="I12" s="15">
-        <v>609218</v>
+        <v>413746</v>
       </c>
       <c r="J12" s="15">
-        <v>413746</v>
+        <v>288089</v>
       </c>
       <c r="K12" s="15">
-        <v>288089</v>
+        <v>382540</v>
       </c>
       <c r="L12" s="15">
-        <v>382540</v>
+        <v>452640</v>
       </c>
       <c r="M12" s="15">
-        <v>452640</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+        <v>794168</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>28</v>
       </c>
@@ -997,142 +996,142 @@
         <v>0</v>
       </c>
       <c r="E13" s="11">
-        <v>0</v>
+        <v>6854</v>
       </c>
       <c r="F13" s="11">
-        <v>6854</v>
+        <v>87750</v>
       </c>
       <c r="G13" s="11">
-        <v>87750</v>
+        <v>90212</v>
       </c>
       <c r="H13" s="11">
-        <v>90212</v>
+        <v>113718</v>
       </c>
       <c r="I13" s="11">
-        <v>113718</v>
+        <v>0</v>
       </c>
       <c r="J13" s="11">
-        <v>0</v>
+        <v>24338</v>
       </c>
       <c r="K13" s="11">
-        <v>24338</v>
+        <v>64519</v>
       </c>
       <c r="L13" s="11">
-        <v>64519</v>
+        <v>44504</v>
       </c>
       <c r="M13" s="11">
-        <v>44504</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+        <v>23011</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15">
-        <v>940613</v>
+        <v>712029</v>
       </c>
       <c r="E14" s="15">
-        <v>712029</v>
+        <v>1933504</v>
       </c>
       <c r="F14" s="15">
-        <v>1933504</v>
+        <v>1743093</v>
       </c>
       <c r="G14" s="15">
-        <v>1743093</v>
+        <v>1265263</v>
       </c>
       <c r="H14" s="15">
-        <v>1265263</v>
+        <v>3057037</v>
       </c>
       <c r="I14" s="15">
-        <v>3057037</v>
+        <v>6858234</v>
       </c>
       <c r="J14" s="15">
-        <v>6858234</v>
+        <v>6773004</v>
       </c>
       <c r="K14" s="15">
-        <v>6773004</v>
+        <v>3227048</v>
       </c>
       <c r="L14" s="15">
-        <v>3227048</v>
+        <v>7614186</v>
       </c>
       <c r="M14" s="15">
-        <v>7614186</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+        <v>12290587</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11">
-        <v>5185616</v>
+        <v>7092127</v>
       </c>
       <c r="E15" s="11">
-        <v>7092127</v>
+        <v>8449553</v>
       </c>
       <c r="F15" s="11">
-        <v>8449553</v>
+        <v>9512459</v>
       </c>
       <c r="G15" s="11">
-        <v>9512459</v>
+        <v>10396124</v>
       </c>
       <c r="H15" s="11">
-        <v>10396124</v>
+        <v>13331972</v>
       </c>
       <c r="I15" s="11">
-        <v>13331972</v>
+        <v>11830439</v>
       </c>
       <c r="J15" s="11">
-        <v>11830439</v>
+        <v>11912435</v>
       </c>
       <c r="K15" s="11">
-        <v>11912435</v>
+        <v>12109951</v>
       </c>
       <c r="L15" s="11">
-        <v>12109951</v>
+        <v>12352314</v>
       </c>
       <c r="M15" s="11">
-        <v>12352314</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+        <v>12248428</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15">
-        <v>1303371</v>
+        <v>2241737</v>
       </c>
       <c r="E16" s="15">
-        <v>2241737</v>
+        <v>1437849</v>
       </c>
       <c r="F16" s="15">
-        <v>1437849</v>
+        <v>2412663</v>
       </c>
       <c r="G16" s="15">
-        <v>2412663</v>
+        <v>2747393</v>
       </c>
       <c r="H16" s="15">
-        <v>2747393</v>
+        <v>1764284</v>
       </c>
       <c r="I16" s="15">
-        <v>1764284</v>
+        <v>1954210</v>
       </c>
       <c r="J16" s="15">
-        <v>1954210</v>
+        <v>1327604</v>
       </c>
       <c r="K16" s="15">
-        <v>1327604</v>
+        <v>2822443</v>
       </c>
       <c r="L16" s="15">
-        <v>2822443</v>
+        <v>2133486</v>
       </c>
       <c r="M16" s="15">
-        <v>2133486</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+        <v>756029</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
@@ -1168,43 +1167,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17">
-        <v>7916436</v>
+        <v>10697657</v>
       </c>
       <c r="E18" s="17">
-        <v>10697657</v>
+        <v>13897736</v>
       </c>
       <c r="F18" s="17">
-        <v>13897736</v>
+        <v>14213339</v>
       </c>
       <c r="G18" s="17">
-        <v>14213339</v>
+        <v>14748755</v>
       </c>
       <c r="H18" s="17">
-        <v>14748755</v>
+        <v>18876229</v>
       </c>
       <c r="I18" s="17">
-        <v>18876229</v>
+        <v>21056629</v>
       </c>
       <c r="J18" s="17">
-        <v>21056629</v>
+        <v>20325470</v>
       </c>
       <c r="K18" s="17">
-        <v>20325470</v>
+        <v>18606501</v>
       </c>
       <c r="L18" s="17">
-        <v>18606501</v>
+        <v>22597130</v>
       </c>
       <c r="M18" s="17">
-        <v>22597130</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+        <v>26112223</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>34</v>
       </c>
@@ -1240,34 +1239,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15">
-        <v>57018</v>
+        <v>209235</v>
       </c>
       <c r="E20" s="15">
-        <v>209235</v>
+        <v>57078</v>
       </c>
       <c r="F20" s="15">
+        <v>57047</v>
+      </c>
+      <c r="G20" s="15">
+        <v>57159</v>
+      </c>
+      <c r="H20" s="15">
         <v>57078</v>
-      </c>
-      <c r="G20" s="15">
-        <v>57047</v>
-      </c>
-      <c r="H20" s="15">
-        <v>57159</v>
       </c>
       <c r="I20" s="15">
         <v>57078</v>
       </c>
       <c r="J20" s="15">
+        <v>80283</v>
+      </c>
+      <c r="K20" s="15">
         <v>57078</v>
-      </c>
-      <c r="K20" s="15">
-        <v>80283</v>
       </c>
       <c r="L20" s="15">
         <v>57078</v>
@@ -1276,7 +1275,7 @@
         <v>57078</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>36</v>
       </c>
@@ -1312,79 +1311,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15">
-        <v>480540</v>
+        <v>476801</v>
       </c>
       <c r="E22" s="15">
-        <v>476801</v>
+        <v>518331</v>
       </c>
       <c r="F22" s="15">
-        <v>518331</v>
+        <v>424911</v>
       </c>
       <c r="G22" s="15">
-        <v>424911</v>
+        <v>587490</v>
       </c>
       <c r="H22" s="15">
-        <v>587490</v>
+        <v>655117</v>
       </c>
       <c r="I22" s="15">
-        <v>655117</v>
+        <v>14474253</v>
       </c>
       <c r="J22" s="15">
-        <v>14474253</v>
+        <v>14530714</v>
       </c>
       <c r="K22" s="15">
-        <v>14530714</v>
+        <v>14475417</v>
       </c>
       <c r="L22" s="15">
-        <v>14475417</v>
+        <v>14589104</v>
       </c>
       <c r="M22" s="15">
-        <v>14589104</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+        <v>14649787</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11">
-        <v>5969</v>
+        <v>5901</v>
       </c>
       <c r="E23" s="11">
-        <v>5901</v>
+        <v>6153</v>
       </c>
       <c r="F23" s="11">
-        <v>6153</v>
+        <v>6245</v>
       </c>
       <c r="G23" s="11">
-        <v>6245</v>
+        <v>5849</v>
       </c>
       <c r="H23" s="11">
-        <v>5849</v>
+        <v>5371</v>
       </c>
       <c r="I23" s="11">
-        <v>5371</v>
+        <v>6278</v>
       </c>
       <c r="J23" s="11">
-        <v>6278</v>
+        <v>5869</v>
       </c>
       <c r="K23" s="11">
-        <v>5869</v>
+        <v>5459</v>
       </c>
       <c r="L23" s="11">
-        <v>5459</v>
+        <v>5056</v>
       </c>
       <c r="M23" s="11">
-        <v>5056</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+        <v>4458</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
         <v>39</v>
       </c>
@@ -1420,115 +1419,115 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11">
-        <v>3454</v>
+        <v>2397</v>
       </c>
       <c r="E25" s="11">
+        <v>2396</v>
+      </c>
+      <c r="F25" s="11">
+        <v>3990</v>
+      </c>
+      <c r="G25" s="11">
+        <v>29136</v>
+      </c>
+      <c r="H25" s="11">
+        <v>15301</v>
+      </c>
+      <c r="I25" s="11">
+        <v>19075</v>
+      </c>
+      <c r="J25" s="11">
+        <v>19414</v>
+      </c>
+      <c r="K25" s="11">
+        <v>8747</v>
+      </c>
+      <c r="L25" s="11">
+        <v>11620</v>
+      </c>
+      <c r="M25" s="11">
         <v>2397</v>
       </c>
-      <c r="F25" s="11">
-        <v>2396</v>
-      </c>
-      <c r="G25" s="11">
-        <v>3990</v>
-      </c>
-      <c r="H25" s="11">
-        <v>29136</v>
-      </c>
-      <c r="I25" s="11">
-        <v>15301</v>
-      </c>
-      <c r="J25" s="11">
-        <v>19075</v>
-      </c>
-      <c r="K25" s="11">
-        <v>19414</v>
-      </c>
-      <c r="L25" s="11">
-        <v>8747</v>
-      </c>
-      <c r="M25" s="11">
-        <v>11620</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17">
-        <v>546981</v>
+        <v>694334</v>
       </c>
       <c r="E26" s="17">
-        <v>694334</v>
+        <v>583958</v>
       </c>
       <c r="F26" s="17">
-        <v>583958</v>
+        <v>492193</v>
       </c>
       <c r="G26" s="17">
-        <v>492193</v>
+        <v>679634</v>
       </c>
       <c r="H26" s="17">
-        <v>679634</v>
+        <v>732867</v>
       </c>
       <c r="I26" s="17">
-        <v>732867</v>
+        <v>14556684</v>
       </c>
       <c r="J26" s="17">
-        <v>14556684</v>
+        <v>14636280</v>
       </c>
       <c r="K26" s="17">
-        <v>14636280</v>
+        <v>14546701</v>
       </c>
       <c r="L26" s="17">
-        <v>14546701</v>
+        <v>14662858</v>
       </c>
       <c r="M26" s="17">
-        <v>14662858</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+        <v>14713720</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="18" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19">
-        <v>8463417</v>
+        <v>11391991</v>
       </c>
       <c r="E27" s="19">
-        <v>11391991</v>
+        <v>14481694</v>
       </c>
       <c r="F27" s="19">
-        <v>14481694</v>
+        <v>14705532</v>
       </c>
       <c r="G27" s="19">
-        <v>14705532</v>
+        <v>15428389</v>
       </c>
       <c r="H27" s="19">
-        <v>15428389</v>
+        <v>19609096</v>
       </c>
       <c r="I27" s="19">
-        <v>19609096</v>
+        <v>35613313</v>
       </c>
       <c r="J27" s="19">
-        <v>35613313</v>
+        <v>34961750</v>
       </c>
       <c r="K27" s="19">
-        <v>34961750</v>
+        <v>33153202</v>
       </c>
       <c r="L27" s="19">
-        <v>33153202</v>
+        <v>37259988</v>
       </c>
       <c r="M27" s="19">
-        <v>37259988</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <v>40825943</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>44</v>
       </c>
@@ -1544,43 +1543,43 @@
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15">
-        <v>2318733</v>
+        <v>1149545</v>
       </c>
       <c r="E29" s="15">
-        <v>1149545</v>
+        <v>2596713</v>
       </c>
       <c r="F29" s="15">
-        <v>2596713</v>
+        <v>2944822</v>
       </c>
       <c r="G29" s="15">
-        <v>2944822</v>
+        <v>1610043</v>
       </c>
       <c r="H29" s="15">
-        <v>1610043</v>
+        <v>3304684</v>
       </c>
       <c r="I29" s="15">
-        <v>3304684</v>
+        <v>3181338</v>
       </c>
       <c r="J29" s="15">
-        <v>3181338</v>
+        <v>1945700</v>
       </c>
       <c r="K29" s="15">
-        <v>1945700</v>
+        <v>3955809</v>
       </c>
       <c r="L29" s="15">
-        <v>3955809</v>
+        <v>3607926</v>
       </c>
       <c r="M29" s="15">
-        <v>3607926</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+        <v>3943868</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>46</v>
       </c>
@@ -1616,151 +1615,151 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15">
-        <v>81231</v>
+        <v>122757</v>
       </c>
       <c r="E31" s="15">
-        <v>122757</v>
+        <v>65349</v>
       </c>
       <c r="F31" s="15">
-        <v>65349</v>
+        <v>122242</v>
       </c>
       <c r="G31" s="15">
-        <v>122242</v>
+        <v>95613</v>
       </c>
       <c r="H31" s="15">
-        <v>95613</v>
+        <v>1159660</v>
       </c>
       <c r="I31" s="15">
-        <v>1159660</v>
+        <v>933730</v>
       </c>
       <c r="J31" s="15">
-        <v>933730</v>
+        <v>71861</v>
       </c>
       <c r="K31" s="15">
-        <v>71861</v>
+        <v>371121</v>
       </c>
       <c r="L31" s="15">
-        <v>371121</v>
+        <v>1787744</v>
       </c>
       <c r="M31" s="15">
-        <v>1787744</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+        <v>224878</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11">
-        <v>803684</v>
+        <v>1025694</v>
       </c>
       <c r="E32" s="11">
-        <v>1025694</v>
+        <v>1411831</v>
       </c>
       <c r="F32" s="11">
-        <v>1411831</v>
+        <v>1623345</v>
       </c>
       <c r="G32" s="11">
-        <v>1623345</v>
+        <v>1152308</v>
       </c>
       <c r="H32" s="11">
-        <v>1152308</v>
+        <v>1294928</v>
       </c>
       <c r="I32" s="11">
-        <v>1294928</v>
+        <v>1284539</v>
       </c>
       <c r="J32" s="11">
-        <v>1284539</v>
+        <v>1397342</v>
       </c>
       <c r="K32" s="11">
-        <v>1397342</v>
+        <v>1289807</v>
       </c>
       <c r="L32" s="11">
-        <v>1289807</v>
+        <v>1330294</v>
       </c>
       <c r="M32" s="11">
-        <v>1330294</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+        <v>2346980</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15">
-        <v>640797</v>
+        <v>2600796</v>
       </c>
       <c r="E33" s="15">
-        <v>2600796</v>
+        <v>2364400</v>
       </c>
       <c r="F33" s="15">
-        <v>2364400</v>
+        <v>1438990</v>
       </c>
       <c r="G33" s="15">
-        <v>1438990</v>
+        <v>31614</v>
       </c>
       <c r="H33" s="15">
-        <v>31614</v>
+        <v>5121595</v>
       </c>
       <c r="I33" s="15">
-        <v>5121595</v>
+        <v>4463121</v>
       </c>
       <c r="J33" s="15">
-        <v>4463121</v>
+        <v>4462588</v>
       </c>
       <c r="K33" s="15">
-        <v>4462588</v>
+        <v>54287</v>
       </c>
       <c r="L33" s="15">
-        <v>54287</v>
+        <v>4056112</v>
       </c>
       <c r="M33" s="15">
-        <v>4056112</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+        <v>4054860</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11">
-        <v>247564</v>
+        <v>3679965</v>
       </c>
       <c r="E34" s="11">
-        <v>3679965</v>
+        <v>3395773</v>
       </c>
       <c r="F34" s="11">
-        <v>3395773</v>
+        <v>2451422</v>
       </c>
       <c r="G34" s="11">
-        <v>2451422</v>
+        <v>5086472</v>
       </c>
       <c r="H34" s="11">
-        <v>5086472</v>
+        <v>5251761</v>
       </c>
       <c r="I34" s="11">
-        <v>5251761</v>
+        <v>6904036</v>
       </c>
       <c r="J34" s="11">
-        <v>6904036</v>
+        <v>6504042</v>
       </c>
       <c r="K34" s="11">
-        <v>6504042</v>
+        <v>6770390</v>
       </c>
       <c r="L34" s="11">
-        <v>6770390</v>
+        <v>8218517</v>
       </c>
       <c r="M34" s="11">
-        <v>8218517</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+        <v>8230314</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>51</v>
       </c>
@@ -1775,28 +1774,28 @@
         <v>0</v>
       </c>
       <c r="G35" s="15">
-        <v>0</v>
+        <v>88966</v>
       </c>
       <c r="H35" s="15">
-        <v>88966</v>
+        <v>0</v>
       </c>
       <c r="I35" s="15">
-        <v>0</v>
+        <v>65011</v>
       </c>
       <c r="J35" s="15">
-        <v>65011</v>
+        <v>66163</v>
       </c>
       <c r="K35" s="15">
-        <v>66163</v>
+        <v>199447</v>
       </c>
       <c r="L35" s="15">
-        <v>199447</v>
+        <v>225271</v>
       </c>
       <c r="M35" s="15">
-        <v>225271</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+        <v>314234</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>52</v>
       </c>
@@ -1832,43 +1831,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17">
-        <v>4092009</v>
+        <v>8578757</v>
       </c>
       <c r="E37" s="17">
-        <v>8578757</v>
+        <v>9834066</v>
       </c>
       <c r="F37" s="17">
-        <v>9834066</v>
+        <v>8580821</v>
       </c>
       <c r="G37" s="17">
-        <v>8580821</v>
+        <v>8065016</v>
       </c>
       <c r="H37" s="17">
-        <v>8065016</v>
+        <v>16132628</v>
       </c>
       <c r="I37" s="17">
-        <v>16132628</v>
+        <v>16831775</v>
       </c>
       <c r="J37" s="17">
-        <v>16831775</v>
+        <v>14447696</v>
       </c>
       <c r="K37" s="17">
-        <v>14447696</v>
+        <v>12640861</v>
       </c>
       <c r="L37" s="17">
-        <v>12640861</v>
+        <v>19225864</v>
       </c>
       <c r="M37" s="17">
-        <v>19225864</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+        <v>19115134</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
         <v>54</v>
       </c>
@@ -1904,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="14" t="s">
         <v>55</v>
       </c>
@@ -1940,7 +1939,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>56</v>
       </c>
@@ -1973,118 +1972,118 @@
         <v>0</v>
       </c>
       <c r="M40" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15">
-        <v>89520</v>
+        <v>90246</v>
       </c>
       <c r="E41" s="15">
-        <v>90246</v>
+        <v>84914</v>
       </c>
       <c r="F41" s="15">
-        <v>84914</v>
+        <v>124378</v>
       </c>
       <c r="G41" s="15">
-        <v>124378</v>
+        <v>124669</v>
       </c>
       <c r="H41" s="15">
-        <v>124669</v>
+        <v>127041</v>
       </c>
       <c r="I41" s="15">
-        <v>127041</v>
+        <v>126538</v>
       </c>
       <c r="J41" s="15">
-        <v>126538</v>
+        <v>176783</v>
       </c>
       <c r="K41" s="15">
-        <v>176783</v>
+        <v>182313</v>
       </c>
       <c r="L41" s="15">
-        <v>182313</v>
+        <v>192456</v>
       </c>
       <c r="M41" s="15">
-        <v>192456</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+        <v>194052</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19">
-        <v>89520</v>
+        <v>90246</v>
       </c>
       <c r="E42" s="19">
-        <v>90246</v>
+        <v>84914</v>
       </c>
       <c r="F42" s="19">
-        <v>84914</v>
+        <v>124378</v>
       </c>
       <c r="G42" s="19">
-        <v>124378</v>
+        <v>124669</v>
       </c>
       <c r="H42" s="19">
-        <v>124669</v>
+        <v>127041</v>
       </c>
       <c r="I42" s="19">
-        <v>127041</v>
+        <v>126538</v>
       </c>
       <c r="J42" s="19">
-        <v>126538</v>
+        <v>176783</v>
       </c>
       <c r="K42" s="19">
-        <v>176783</v>
+        <v>182313</v>
       </c>
       <c r="L42" s="19">
-        <v>182313</v>
+        <v>192456</v>
       </c>
       <c r="M42" s="19">
-        <v>192456</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+        <v>1194052</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17">
-        <v>4181529</v>
+        <v>8669003</v>
       </c>
       <c r="E43" s="17">
-        <v>8669003</v>
+        <v>9918980</v>
       </c>
       <c r="F43" s="17">
-        <v>9918980</v>
+        <v>8705199</v>
       </c>
       <c r="G43" s="17">
-        <v>8705199</v>
+        <v>8189685</v>
       </c>
       <c r="H43" s="17">
-        <v>8189685</v>
+        <v>16259669</v>
       </c>
       <c r="I43" s="17">
-        <v>16259669</v>
+        <v>16958313</v>
       </c>
       <c r="J43" s="17">
-        <v>16958313</v>
+        <v>14624479</v>
       </c>
       <c r="K43" s="17">
-        <v>14624479</v>
+        <v>12823174</v>
       </c>
       <c r="L43" s="17">
-        <v>12823174</v>
+        <v>19418320</v>
       </c>
       <c r="M43" s="17">
-        <v>19418320</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+        <v>20309186</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="12" t="s">
         <v>60</v>
       </c>
@@ -2100,7 +2099,7 @@
       <c r="L44" s="13"/>
       <c r="M44" s="13"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>61</v>
       </c>
@@ -2121,7 +2120,7 @@
         <v>680400</v>
       </c>
       <c r="I45" s="15">
-        <v>680400</v>
+        <v>14288400</v>
       </c>
       <c r="J45" s="15">
         <v>14288400</v>
@@ -2136,7 +2135,7 @@
         <v>14288400</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -2172,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" s="14" t="s">
         <v>63</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>64</v>
       </c>
@@ -2217,34 +2216,34 @@
         <v>0</v>
       </c>
       <c r="E48" s="11">
-        <v>0</v>
+        <v>-222366</v>
       </c>
       <c r="F48" s="11">
-        <v>-222366</v>
+        <v>-103447</v>
       </c>
       <c r="G48" s="11">
-        <v>-103447</v>
+        <v>-135553</v>
       </c>
       <c r="H48" s="11">
-        <v>-135553</v>
+        <v>-107912</v>
       </c>
       <c r="I48" s="11">
-        <v>-107912</v>
+        <v>-245457</v>
       </c>
       <c r="J48" s="11">
-        <v>-245457</v>
+        <v>-161217</v>
       </c>
       <c r="K48" s="11">
-        <v>-161217</v>
+        <v>-129985</v>
       </c>
       <c r="L48" s="11">
-        <v>-129985</v>
+        <v>-149562</v>
       </c>
       <c r="M48" s="11">
-        <v>-149562</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+        <v>-220810</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
         <v>65</v>
       </c>
@@ -2256,16 +2255,16 @@
         <v>0</v>
       </c>
       <c r="F49" s="15">
-        <v>0</v>
+        <v>-28832</v>
       </c>
       <c r="G49" s="15">
-        <v>-28832</v>
+        <v>3795</v>
       </c>
       <c r="H49" s="15">
-        <v>3795</v>
+        <v>2748</v>
       </c>
       <c r="I49" s="15">
-        <v>2748</v>
+        <v>0</v>
       </c>
       <c r="J49" s="15">
         <v>0</v>
@@ -2277,10 +2276,10 @@
         <v>0</v>
       </c>
       <c r="M49" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+        <v>6131</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="10" t="s">
         <v>66</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>68040</v>
       </c>
       <c r="K50" s="11">
-        <v>68040</v>
+        <v>287653</v>
       </c>
       <c r="L50" s="11">
         <v>287653</v>
@@ -2316,7 +2315,7 @@
         <v>287653</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
         <v>67</v>
       </c>
@@ -2352,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>68</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>69</v>
       </c>
@@ -2409,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="I53" s="15">
-        <v>0</v>
+        <v>187202</v>
       </c>
       <c r="J53" s="15">
         <v>187202</v>
@@ -2424,7 +2423,7 @@
         <v>187202</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>70</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="14" t="s">
         <v>71</v>
       </c>
@@ -2496,115 +2495,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11">
-        <v>3533448</v>
+        <v>1974548</v>
       </c>
       <c r="E56" s="11">
-        <v>1974548</v>
+        <v>4036640</v>
       </c>
       <c r="F56" s="11">
-        <v>4036640</v>
+        <v>5384172</v>
       </c>
       <c r="G56" s="11">
-        <v>5384172</v>
+        <v>6622022</v>
       </c>
       <c r="H56" s="11">
-        <v>6622022</v>
+        <v>2706151</v>
       </c>
       <c r="I56" s="11">
-        <v>2706151</v>
+        <v>4356815</v>
       </c>
       <c r="J56" s="11">
-        <v>4356815</v>
+        <v>5954846</v>
       </c>
       <c r="K56" s="11">
-        <v>5954846</v>
+        <v>5696758</v>
       </c>
       <c r="L56" s="11">
-        <v>5696758</v>
+        <v>3227975</v>
       </c>
       <c r="M56" s="11">
-        <v>3227975</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+        <v>5968181</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17">
-        <v>4281888</v>
+        <v>2722988</v>
       </c>
       <c r="E57" s="17">
-        <v>2722988</v>
+        <v>4562714</v>
       </c>
       <c r="F57" s="17">
-        <v>4562714</v>
+        <v>6000333</v>
       </c>
       <c r="G57" s="17">
-        <v>6000333</v>
+        <v>7238704</v>
       </c>
       <c r="H57" s="17">
-        <v>7238704</v>
+        <v>3349427</v>
       </c>
       <c r="I57" s="17">
-        <v>3349427</v>
+        <v>18655000</v>
       </c>
       <c r="J57" s="17">
-        <v>18655000</v>
+        <v>20337271</v>
       </c>
       <c r="K57" s="17">
-        <v>20337271</v>
+        <v>20330028</v>
       </c>
       <c r="L57" s="17">
-        <v>20330028</v>
+        <v>17841668</v>
       </c>
       <c r="M57" s="17">
-        <v>17841668</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+        <v>20516757</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19">
-        <v>8463417</v>
+        <v>11391991</v>
       </c>
       <c r="E58" s="19">
-        <v>11391991</v>
+        <v>14481694</v>
       </c>
       <c r="F58" s="19">
-        <v>14481694</v>
+        <v>14705532</v>
       </c>
       <c r="G58" s="19">
-        <v>14705532</v>
+        <v>15428389</v>
       </c>
       <c r="H58" s="19">
-        <v>15428389</v>
+        <v>19609096</v>
       </c>
       <c r="I58" s="19">
-        <v>19609096</v>
+        <v>35613313</v>
       </c>
       <c r="J58" s="19">
-        <v>35613313</v>
+        <v>34961750</v>
       </c>
       <c r="K58" s="19">
-        <v>34961750</v>
+        <v>33153202</v>
       </c>
       <c r="L58" s="19">
-        <v>33153202</v>
+        <v>37259988</v>
       </c>
       <c r="M58" s="19">
-        <v>37259988</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+        <v>40825943</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>

</xml_diff>